<commit_message>
Study 1 model fitting results
</commit_message>
<xml_diff>
--- a/Study 1 model fitting results.xlsx
+++ b/Study 1 model fitting results.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimi/Desktop/Desktop Contents/Dissertation/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BCCE7F-7B82-3842-B51A-B24B1F63FC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B2CCF3-8016-5F49-B7EF-162B6AB64722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="520" windowWidth="47040" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55640" yWindow="3740" windowWidth="47040" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Result_PSTRE" sheetId="13" r:id="rId1"/>
-    <sheet name="Result_LITNUM" sheetId="3" r:id="rId2"/>
-    <sheet name="PSTRE_ranef_pv1" sheetId="19" r:id="rId3"/>
-    <sheet name="LITNUM_ranef_pv1" sheetId="18" r:id="rId4"/>
-    <sheet name="PSTRE PVs" sheetId="12" r:id="rId5"/>
-    <sheet name="LITNUM PVs" sheetId="16" r:id="rId6"/>
-    <sheet name="Model AIC comparison" sheetId="8" r:id="rId7"/>
-    <sheet name="Null model" sheetId="2" r:id="rId8"/>
+    <sheet name="Study 1 result" sheetId="21" r:id="rId1"/>
+    <sheet name="Study 1 result_raw" sheetId="20" r:id="rId2"/>
+    <sheet name="Result_PSTRE" sheetId="13" r:id="rId3"/>
+    <sheet name="Result_LITNUM" sheetId="3" r:id="rId4"/>
+    <sheet name="PSTRE_ranef_pv1" sheetId="19" r:id="rId5"/>
+    <sheet name="LITNUM_ranef_pv1" sheetId="18" r:id="rId6"/>
+    <sheet name="PSTRE PVs" sheetId="12" r:id="rId7"/>
+    <sheet name="LITNUM PVs" sheetId="16" r:id="rId8"/>
+    <sheet name="Model AIC comparison" sheetId="8" r:id="rId9"/>
+    <sheet name="Null model" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3699" uniqueCount="740">
   <si>
     <t>.</t>
   </si>
@@ -2255,6 +2257,227 @@
   <si>
     <t># of observations = 35,248, # of countries = 35</t>
   </si>
+  <si>
+    <t>Literacy + Numeracy Final Model</t>
+  </si>
+  <si>
+    <t>PSTRE Final Model</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>95% CIs</t>
+  </si>
+  <si>
+    <t>Exp(Estimate)</t>
+  </si>
+  <si>
+    <t>Exp(95% CIs)</t>
+  </si>
+  <si>
+    <t>[-0.139, 0.563]</t>
+  </si>
+  <si>
+    <t>[0.870, 1.756]</t>
+  </si>
+  <si>
+    <t>[-0.144, 0.710]</t>
+  </si>
+  <si>
+    <t>[0.866, 2.035]</t>
+  </si>
+  <si>
+    <t>Literacy + Numeracy/PSTRE</t>
+  </si>
+  <si>
+    <t>[0.040, 0.178]</t>
+  </si>
+  <si>
+    <t>[1.041, 1.194]</t>
+  </si>
+  <si>
+    <t>[-0.055, 0.097]</t>
+  </si>
+  <si>
+    <t>[0.946, 1.102]</t>
+  </si>
+  <si>
+    <t>[0.252, 0.502]</t>
+  </si>
+  <si>
+    <t>[1.286, 1.653]</t>
+  </si>
+  <si>
+    <t>[0.263, 0.509]</t>
+  </si>
+  <si>
+    <t>[1.300, 1.664]</t>
+  </si>
+  <si>
+    <t>[-0.354, -0.178]</t>
+  </si>
+  <si>
+    <t>[0.702, 0.837]</t>
+  </si>
+  <si>
+    <t>[-0.399, -0.195]</t>
+  </si>
+  <si>
+    <t>[0.671, 0.823]</t>
+  </si>
+  <si>
+    <t>[-0.027, 0.161]</t>
+  </si>
+  <si>
+    <t>[0.973, 1.175]</t>
+  </si>
+  <si>
+    <t>[0.017, 0.229]</t>
+  </si>
+  <si>
+    <t>[1.017, 1.257]</t>
+  </si>
+  <si>
+    <t>[0.245, 0.869]</t>
+  </si>
+  <si>
+    <t>[1.278, 2.384]</t>
+  </si>
+  <si>
+    <t>[0.083, 0.851]</t>
+  </si>
+  <si>
+    <t>[1.086, 2.342]</t>
+  </si>
+  <si>
+    <t>[-0.08, 0.528]</t>
+  </si>
+  <si>
+    <t>[0.923, 1.695]</t>
+  </si>
+  <si>
+    <t>[-0.303, 0.453]</t>
+  </si>
+  <si>
+    <t>[0.738, 1.573]</t>
+  </si>
+  <si>
+    <t>[-0.087, 0.579]</t>
+  </si>
+  <si>
+    <t>[0.916, 1.785]</t>
+  </si>
+  <si>
+    <t>[-0.271, 0.541]</t>
+  </si>
+  <si>
+    <t>[0.763, 1.717]</t>
+  </si>
+  <si>
+    <t>[0.436, 0.604]</t>
+  </si>
+  <si>
+    <t>[1.546, 1.830]</t>
+  </si>
+  <si>
+    <t>[0.465, 0.657]</t>
+  </si>
+  <si>
+    <t>[1.592, 1.929]</t>
+  </si>
+  <si>
+    <t>[0.157, 0.181]</t>
+  </si>
+  <si>
+    <t>[1.170, 1.198]</t>
+  </si>
+  <si>
+    <t>[0.153, 0.181]</t>
+  </si>
+  <si>
+    <t>[1.166, 1.198]</t>
+  </si>
+  <si>
+    <t>[-0.475, -0.145]</t>
+  </si>
+  <si>
+    <t>[0.622, 0.865]</t>
+  </si>
+  <si>
+    <t>[-0.450, -0.050]</t>
+  </si>
+  <si>
+    <t>[0.638, 0.951]</t>
+  </si>
+  <si>
+    <t>[0.261, 0.531]</t>
+  </si>
+  <si>
+    <t>[1.298, 1.701]</t>
+  </si>
+  <si>
+    <t>[0.358, 0.664]</t>
+  </si>
+  <si>
+    <t>[1.431, 1.942]</t>
+  </si>
+  <si>
+    <t>[-0.160, 0.094]</t>
+  </si>
+  <si>
+    <t>[0.852, 1.099]</t>
+  </si>
+  <si>
+    <t>[-0.087, 0.203]</t>
+  </si>
+  <si>
+    <t>[0.917, 1.225]</t>
+  </si>
+  <si>
+    <t>Study 1- Employability</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Literacy + Numeracy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Final Model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PSTRE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Final Model</t>
+    </r>
+  </si>
+  <si>
+    <t>Study 1 - Employability</t>
+  </si>
 </sst>
 </file>
 
@@ -2266,7 +2489,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2424,8 +2647,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2456,8 +2698,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2485,6 +2739,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2497,7 +2837,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2757,6 +3097,211 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3083,10 +3628,1319 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E6F793-F5A6-DA4D-9708-7D89CE3448CB}">
+  <dimension ref="A2:I22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" style="145" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="145" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="145" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" style="146" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="146" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="146" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" s="112" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="147" t="s">
+        <v>736</v>
+      </c>
+      <c r="B2" s="149" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="152" t="s">
+        <v>738</v>
+      </c>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+    </row>
+    <row r="3" spans="1:9" s="120" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="148"/>
+      <c r="B3" s="113" t="s">
+        <v>679</v>
+      </c>
+      <c r="C3" s="114" t="s">
+        <v>680</v>
+      </c>
+      <c r="D3" s="115" t="s">
+        <v>681</v>
+      </c>
+      <c r="E3" s="116" t="s">
+        <v>682</v>
+      </c>
+      <c r="F3" s="117" t="s">
+        <v>679</v>
+      </c>
+      <c r="G3" s="118" t="s">
+        <v>680</v>
+      </c>
+      <c r="H3" s="119" t="s">
+        <v>681</v>
+      </c>
+      <c r="I3" s="119" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="121" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="122"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+    </row>
+    <row r="5" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="130" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="131" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="132">
+        <v>1.2361478850785035</v>
+      </c>
+      <c r="E5" s="133" t="s">
+        <v>684</v>
+      </c>
+      <c r="F5" s="134" t="s">
+        <v>408</v>
+      </c>
+      <c r="G5" s="135" t="s">
+        <v>685</v>
+      </c>
+      <c r="H5" s="136">
+        <v>1.3271051618171572</v>
+      </c>
+      <c r="I5" s="136" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="129" t="s">
+        <v>687</v>
+      </c>
+      <c r="B6" s="130" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" s="131" t="s">
+        <v>688</v>
+      </c>
+      <c r="D6" s="132">
+        <v>1.1151623503414478</v>
+      </c>
+      <c r="E6" s="133" t="s">
+        <v>689</v>
+      </c>
+      <c r="F6" s="134" t="s">
+        <v>409</v>
+      </c>
+      <c r="G6" s="135" t="s">
+        <v>690</v>
+      </c>
+      <c r="H6" s="136">
+        <v>1.0212220516375285</v>
+      </c>
+      <c r="I6" s="136" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="129" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="130" t="s">
+        <v>568</v>
+      </c>
+      <c r="C7" s="131" t="s">
+        <v>692</v>
+      </c>
+      <c r="D7" s="132">
+        <v>1.4579043093712258</v>
+      </c>
+      <c r="E7" s="133" t="s">
+        <v>693</v>
+      </c>
+      <c r="F7" s="134" t="s">
+        <v>410</v>
+      </c>
+      <c r="G7" s="135" t="s">
+        <v>694</v>
+      </c>
+      <c r="H7" s="136">
+        <v>1.4710846708147431</v>
+      </c>
+      <c r="I7" s="136" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="129" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="130" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="131" t="s">
+        <v>696</v>
+      </c>
+      <c r="D8" s="132">
+        <v>0.76643912750101917</v>
+      </c>
+      <c r="E8" s="133" t="s">
+        <v>697</v>
+      </c>
+      <c r="F8" s="134" t="s">
+        <v>411</v>
+      </c>
+      <c r="G8" s="135" t="s">
+        <v>698</v>
+      </c>
+      <c r="H8" s="136">
+        <v>0.74304401236193984</v>
+      </c>
+      <c r="I8" s="136" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="129" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="130" t="s">
+        <v>569</v>
+      </c>
+      <c r="C9" s="131" t="s">
+        <v>700</v>
+      </c>
+      <c r="D9" s="132">
+        <v>1.0692954781746002</v>
+      </c>
+      <c r="E9" s="133" t="s">
+        <v>701</v>
+      </c>
+      <c r="F9" s="134" t="s">
+        <v>412</v>
+      </c>
+      <c r="G9" s="135" t="s">
+        <v>702</v>
+      </c>
+      <c r="H9" s="136">
+        <v>1.1308844209474893</v>
+      </c>
+      <c r="I9" s="136" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="129" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>570</v>
+      </c>
+      <c r="C10" s="131" t="s">
+        <v>704</v>
+      </c>
+      <c r="D10" s="132">
+        <v>1.7454283529493428</v>
+      </c>
+      <c r="E10" s="133" t="s">
+        <v>705</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>413</v>
+      </c>
+      <c r="G10" s="135" t="s">
+        <v>706</v>
+      </c>
+      <c r="H10" s="136">
+        <v>1.5952014034170006</v>
+      </c>
+      <c r="I10" s="136" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="130" t="s">
+        <v>571</v>
+      </c>
+      <c r="C11" s="131" t="s">
+        <v>708</v>
+      </c>
+      <c r="D11" s="132">
+        <v>1.2510710194283623</v>
+      </c>
+      <c r="E11" s="133" t="s">
+        <v>709</v>
+      </c>
+      <c r="F11" s="134" t="s">
+        <v>414</v>
+      </c>
+      <c r="G11" s="135" t="s">
+        <v>710</v>
+      </c>
+      <c r="H11" s="136">
+        <v>1.0778841508846315</v>
+      </c>
+      <c r="I11" s="136" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="129" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="130" t="s">
+        <v>614</v>
+      </c>
+      <c r="C12" s="131" t="s">
+        <v>712</v>
+      </c>
+      <c r="D12" s="132">
+        <v>1.2788995735417383</v>
+      </c>
+      <c r="E12" s="133" t="s">
+        <v>713</v>
+      </c>
+      <c r="F12" s="134" t="s">
+        <v>415</v>
+      </c>
+      <c r="G12" s="135" t="s">
+        <v>714</v>
+      </c>
+      <c r="H12" s="136">
+        <v>1.1445367843513146</v>
+      </c>
+      <c r="I12" s="136" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="130" t="s">
+        <v>615</v>
+      </c>
+      <c r="C13" s="131" t="s">
+        <v>716</v>
+      </c>
+      <c r="D13" s="132">
+        <v>1.6820276496988864</v>
+      </c>
+      <c r="E13" s="133" t="s">
+        <v>717</v>
+      </c>
+      <c r="F13" s="134" t="s">
+        <v>383</v>
+      </c>
+      <c r="G13" s="135" t="s">
+        <v>718</v>
+      </c>
+      <c r="H13" s="136">
+        <v>1.7524240484244991</v>
+      </c>
+      <c r="I13" s="136" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="129" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="130" t="s">
+        <v>548</v>
+      </c>
+      <c r="C14" s="131" t="s">
+        <v>720</v>
+      </c>
+      <c r="D14" s="132">
+        <v>1.1841201389239695</v>
+      </c>
+      <c r="E14" s="133" t="s">
+        <v>721</v>
+      </c>
+      <c r="F14" s="134" t="s">
+        <v>384</v>
+      </c>
+      <c r="G14" s="135" t="s">
+        <v>722</v>
+      </c>
+      <c r="H14" s="136">
+        <v>1.1817542653083615</v>
+      </c>
+      <c r="I14" s="136" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="129" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="130" t="s">
+        <v>616</v>
+      </c>
+      <c r="C15" s="131" t="s">
+        <v>724</v>
+      </c>
+      <c r="D15" s="132">
+        <v>0.73344695622428924</v>
+      </c>
+      <c r="E15" s="133" t="s">
+        <v>725</v>
+      </c>
+      <c r="F15" s="134" t="s">
+        <v>672</v>
+      </c>
+      <c r="G15" s="135" t="s">
+        <v>726</v>
+      </c>
+      <c r="H15" s="136">
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="I15" s="136" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="129" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="130" t="s">
+        <v>574</v>
+      </c>
+      <c r="C16" s="131" t="s">
+        <v>728</v>
+      </c>
+      <c r="D16" s="132">
+        <v>1.4858693175513897</v>
+      </c>
+      <c r="E16" s="133" t="s">
+        <v>729</v>
+      </c>
+      <c r="F16" s="134" t="s">
+        <v>351</v>
+      </c>
+      <c r="G16" s="135" t="s">
+        <v>730</v>
+      </c>
+      <c r="H16" s="136">
+        <v>1.6669573190640476</v>
+      </c>
+      <c r="I16" s="136" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="129" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="130" t="s">
+        <v>575</v>
+      </c>
+      <c r="C17" s="131" t="s">
+        <v>732</v>
+      </c>
+      <c r="D17" s="132">
+        <v>0.96753855958903201</v>
+      </c>
+      <c r="E17" s="133" t="s">
+        <v>733</v>
+      </c>
+      <c r="F17" s="134" t="s">
+        <v>417</v>
+      </c>
+      <c r="G17" s="135" t="s">
+        <v>734</v>
+      </c>
+      <c r="H17" s="136">
+        <v>1.0597149957102876</v>
+      </c>
+      <c r="I17" s="136" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="121" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="130"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="137"/>
+    </row>
+    <row r="19" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="130" t="s">
+        <v>576</v>
+      </c>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="134" t="s">
+        <v>418</v>
+      </c>
+      <c r="G19" s="127"/>
+      <c r="H19" s="127"/>
+      <c r="I19" s="137"/>
+    </row>
+    <row r="20" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="129" t="s">
+        <v>687</v>
+      </c>
+      <c r="B20" s="130" t="s">
+        <v>577</v>
+      </c>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="134" t="s">
+        <v>419</v>
+      </c>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="137"/>
+    </row>
+    <row r="21" spans="1:9" s="121" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="138" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="139" t="s">
+        <v>578</v>
+      </c>
+      <c r="C21" s="140"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="142" t="s">
+        <v>420</v>
+      </c>
+      <c r="G21" s="143"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="144"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F22" s="104"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="104"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="122.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2772C4AA-3B6B-0743-BCCE-385E9F35E3DE}">
+  <dimension ref="A2:I32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.6640625" style="105" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="89" customWidth="1"/>
+    <col min="3" max="5" width="13.83203125" style="89" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="93" customWidth="1"/>
+    <col min="7" max="9" width="13.83203125" style="93" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="105"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" s="89" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="153" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" s="155" t="s">
+        <v>677</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="156" t="s">
+        <v>678</v>
+      </c>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+    </row>
+    <row r="3" spans="1:9" s="93" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="154"/>
+      <c r="B3" s="90" t="s">
+        <v>679</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>680</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>681</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>682</v>
+      </c>
+      <c r="F3" s="91" t="s">
+        <v>679</v>
+      </c>
+      <c r="G3" s="91" t="s">
+        <v>680</v>
+      </c>
+      <c r="H3" s="91" t="s">
+        <v>681</v>
+      </c>
+      <c r="I3" s="91" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="95"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+    </row>
+    <row r="5" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="98" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="99" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="99">
+        <v>1.2361478850785035</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>684</v>
+      </c>
+      <c r="F5" s="101" t="s">
+        <v>408</v>
+      </c>
+      <c r="G5" s="99" t="s">
+        <v>685</v>
+      </c>
+      <c r="H5" s="99">
+        <v>1.3271051618171572</v>
+      </c>
+      <c r="I5" s="99" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="97" t="s">
+        <v>687</v>
+      </c>
+      <c r="B6" s="98" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" s="99" t="s">
+        <v>688</v>
+      </c>
+      <c r="D6" s="99">
+        <v>1.1151623503414478</v>
+      </c>
+      <c r="E6" s="100" t="s">
+        <v>689</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>409</v>
+      </c>
+      <c r="G6" s="99" t="s">
+        <v>690</v>
+      </c>
+      <c r="H6" s="99">
+        <v>1.0212220516375285</v>
+      </c>
+      <c r="I6" s="99" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="98" t="s">
+        <v>568</v>
+      </c>
+      <c r="C7" s="99" t="s">
+        <v>692</v>
+      </c>
+      <c r="D7" s="99">
+        <v>1.4579043093712258</v>
+      </c>
+      <c r="E7" s="100" t="s">
+        <v>693</v>
+      </c>
+      <c r="F7" s="101" t="s">
+        <v>410</v>
+      </c>
+      <c r="G7" s="99" t="s">
+        <v>694</v>
+      </c>
+      <c r="H7" s="99">
+        <v>1.4710846708147431</v>
+      </c>
+      <c r="I7" s="99" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="98" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>696</v>
+      </c>
+      <c r="D8" s="99">
+        <v>0.76643912750101917</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>697</v>
+      </c>
+      <c r="F8" s="101" t="s">
+        <v>411</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>698</v>
+      </c>
+      <c r="H8" s="99">
+        <v>0.74304401236193984</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="98" t="s">
+        <v>569</v>
+      </c>
+      <c r="C9" s="99" t="s">
+        <v>700</v>
+      </c>
+      <c r="D9" s="99">
+        <v>1.0692954781746002</v>
+      </c>
+      <c r="E9" s="100" t="s">
+        <v>701</v>
+      </c>
+      <c r="F9" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="G9" s="99" t="s">
+        <v>702</v>
+      </c>
+      <c r="H9" s="99">
+        <v>1.1308844209474893</v>
+      </c>
+      <c r="I9" s="99" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="97" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="98" t="s">
+        <v>570</v>
+      </c>
+      <c r="C10" s="99" t="s">
+        <v>704</v>
+      </c>
+      <c r="D10" s="99">
+        <v>1.7454283529493428</v>
+      </c>
+      <c r="E10" s="100" t="s">
+        <v>705</v>
+      </c>
+      <c r="F10" s="101" t="s">
+        <v>413</v>
+      </c>
+      <c r="G10" s="99" t="s">
+        <v>706</v>
+      </c>
+      <c r="H10" s="99">
+        <v>1.5952014034170006</v>
+      </c>
+      <c r="I10" s="99" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="98" t="s">
+        <v>571</v>
+      </c>
+      <c r="C11" s="99" t="s">
+        <v>708</v>
+      </c>
+      <c r="D11" s="99">
+        <v>1.2510710194283623</v>
+      </c>
+      <c r="E11" s="100" t="s">
+        <v>709</v>
+      </c>
+      <c r="F11" s="101" t="s">
+        <v>414</v>
+      </c>
+      <c r="G11" s="99" t="s">
+        <v>710</v>
+      </c>
+      <c r="H11" s="99">
+        <v>1.0778841508846315</v>
+      </c>
+      <c r="I11" s="99" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="97" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="98" t="s">
+        <v>614</v>
+      </c>
+      <c r="C12" s="99" t="s">
+        <v>712</v>
+      </c>
+      <c r="D12" s="99">
+        <v>1.2788995735417383</v>
+      </c>
+      <c r="E12" s="100" t="s">
+        <v>713</v>
+      </c>
+      <c r="F12" s="101" t="s">
+        <v>415</v>
+      </c>
+      <c r="G12" s="99" t="s">
+        <v>714</v>
+      </c>
+      <c r="H12" s="99">
+        <v>1.1445367843513146</v>
+      </c>
+      <c r="I12" s="99" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="97" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="98" t="s">
+        <v>615</v>
+      </c>
+      <c r="C13" s="99" t="s">
+        <v>716</v>
+      </c>
+      <c r="D13" s="99">
+        <v>1.6820276496988864</v>
+      </c>
+      <c r="E13" s="100" t="s">
+        <v>717</v>
+      </c>
+      <c r="F13" s="101" t="s">
+        <v>383</v>
+      </c>
+      <c r="G13" s="99" t="s">
+        <v>718</v>
+      </c>
+      <c r="H13" s="99">
+        <v>1.7524240484244991</v>
+      </c>
+      <c r="I13" s="99" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="98" t="s">
+        <v>548</v>
+      </c>
+      <c r="C14" s="99" t="s">
+        <v>720</v>
+      </c>
+      <c r="D14" s="99">
+        <v>1.1841201389239695</v>
+      </c>
+      <c r="E14" s="100" t="s">
+        <v>721</v>
+      </c>
+      <c r="F14" s="101" t="s">
+        <v>384</v>
+      </c>
+      <c r="G14" s="99" t="s">
+        <v>722</v>
+      </c>
+      <c r="H14" s="99">
+        <v>1.1817542653083615</v>
+      </c>
+      <c r="I14" s="99" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="97" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="98" t="s">
+        <v>616</v>
+      </c>
+      <c r="C15" s="99" t="s">
+        <v>724</v>
+      </c>
+      <c r="D15" s="99">
+        <v>0.73344695622428924</v>
+      </c>
+      <c r="E15" s="100" t="s">
+        <v>725</v>
+      </c>
+      <c r="F15" s="101" t="s">
+        <v>672</v>
+      </c>
+      <c r="G15" s="99" t="s">
+        <v>726</v>
+      </c>
+      <c r="H15" s="99">
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="I15" s="99" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="98" t="s">
+        <v>574</v>
+      </c>
+      <c r="C16" s="99" t="s">
+        <v>728</v>
+      </c>
+      <c r="D16" s="99">
+        <v>1.4858693175513897</v>
+      </c>
+      <c r="E16" s="100" t="s">
+        <v>729</v>
+      </c>
+      <c r="F16" s="101" t="s">
+        <v>351</v>
+      </c>
+      <c r="G16" s="99" t="s">
+        <v>730</v>
+      </c>
+      <c r="H16" s="99">
+        <v>1.6669573190640476</v>
+      </c>
+      <c r="I16" s="99" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="97" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="98" t="s">
+        <v>575</v>
+      </c>
+      <c r="C17" s="99" t="s">
+        <v>732</v>
+      </c>
+      <c r="D17" s="99">
+        <v>0.96753855958903201</v>
+      </c>
+      <c r="E17" s="100" t="s">
+        <v>733</v>
+      </c>
+      <c r="F17" s="101" t="s">
+        <v>417</v>
+      </c>
+      <c r="G17" s="99" t="s">
+        <v>734</v>
+      </c>
+      <c r="H17" s="99">
+        <v>1.0597149957102876</v>
+      </c>
+      <c r="I17" s="99" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="97" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="98"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="101"/>
+    </row>
+    <row r="19" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="97" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="98"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="101"/>
+    </row>
+    <row r="20" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="98"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="101"/>
+    </row>
+    <row r="21" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="98"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="101"/>
+    </row>
+    <row r="22" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="98"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="101"/>
+    </row>
+    <row r="23" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="98"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="101"/>
+    </row>
+    <row r="24" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="97"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="93"/>
+      <c r="I24" s="101"/>
+    </row>
+    <row r="25" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="98"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="101"/>
+    </row>
+    <row r="26" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="98" t="s">
+        <v>576</v>
+      </c>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="101" t="s">
+        <v>418</v>
+      </c>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="I26" s="101"/>
+    </row>
+    <row r="27" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="97" t="s">
+        <v>687</v>
+      </c>
+      <c r="B27" s="98" t="s">
+        <v>577</v>
+      </c>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="101" t="s">
+        <v>419</v>
+      </c>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="101"/>
+    </row>
+    <row r="28" spans="1:9" s="94" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="98" t="s">
+        <v>578</v>
+      </c>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="101" t="s">
+        <v>420</v>
+      </c>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="101"/>
+    </row>
+    <row r="29" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="102"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="104"/>
+      <c r="I29" s="104"/>
+    </row>
+    <row r="30" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="102"/>
+      <c r="E30" s="103"/>
+    </row>
+    <row r="31" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="97"/>
+      <c r="B31" s="102"/>
+      <c r="E31" s="103"/>
+    </row>
+    <row r="32" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="106" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="107">
+        <v>17708.71</v>
+      </c>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="110">
+        <v>13978</v>
+      </c>
+      <c r="G32" s="111"/>
+      <c r="H32" s="111"/>
+      <c r="I32" s="111"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92288717-A2D3-A84E-B27A-83ADB33A2C54}">
   <dimension ref="A2:N43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
@@ -4322,7 +6176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N43"/>
   <sheetViews>
@@ -5547,7 +7401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81D37E6-6627-4133-99E4-C14FF649944B}">
   <dimension ref="A1:D97"/>
   <sheetViews>
@@ -6931,7 +8785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89756970-2E78-4B9C-9CEB-B909697611D3}">
   <dimension ref="A1:D106"/>
   <sheetViews>
@@ -8441,7 +10295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233B1835-794F-E640-BAF0-2B9B5CC81A8F}">
   <dimension ref="A2:AG296"/>
   <sheetViews>
@@ -31365,7 +33219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6663F0AD-AA73-7F47-BC37-069690D7CC4D}">
   <dimension ref="A2:AD296"/>
   <sheetViews>
@@ -53752,7 +55606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2213DAD1-B3D5-444E-BDCC-348C5B712C24}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -53952,127 +55806,4 @@
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A25"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="122.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>